<commit_message>
Update file post correzione errori segnalati
Aggiornamento dei file data.json, report_checklist.xlsx e contenuto FILES a seguito delle segnalazioni ricevute
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111REPLY000000/xenia-reply/appheal-ldo/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111REPLY000000/xenia-reply/appheal-ldo/1.0/report-checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Drive condivisi\Appheal Pubblico\ADT\Crema\LDO\VALIDAZIONE FSE 2.0\ACCREDITAMENTO\VALIDAZIONE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Drive condivisi\Appheal Pubblico\ADT\Crema\LDO\VALIDAZIONE FSE 2.0\ACCREDITAMENTO\GATEWAY\S1#111REPLY000000\xenia-reply\appheal-ldo\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="176">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -835,40 +835,25 @@
     <t>Non gestito</t>
   </si>
   <si>
-    <t>2f3327b7fde1ee27</t>
-  </si>
-  <si>
-    <t>c6cc578239c5f31f</t>
-  </si>
-  <si>
-    <t>a3dcef097f65bdfe</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30209.4.4.60e269b87d60fba262c2039285bebf5d5cc20e076a904a79c3e9889c68310ef8.9c335494a8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30209.4.4.0d3e2592337ef76d524b92555c084fb0ce55b5d728f12ec351813aa5f07662ee.199d3691d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30209.4.4.9584db2851a4b4856fcaf4613426d0c9dcbf8b0e949220c200e75e7db39b0780.49380b0dfd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2032be66b56bf299</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.30209.4.4.f457a70f1d4e9c196437cb83be437f81aad8df36041e1ba88d703dd0bce0c47c.a587f8cfcf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-06-20T12:51:14Z</t>
-  </si>
-  <si>
-    <t>2023-06-20T13:32:48Z</t>
-  </si>
-  <si>
-    <t>2023-06-20T13:40:58Z</t>
-  </si>
-  <si>
     <t>2023-06-20T12:25:45Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30209.4.4.c68fc744e05d8ef909d0c6c865ac0cd7f3f1cf83d20ce5ced6f567e488ff7c94.e4bacc3322^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4151808c071b5442</t>
+  </si>
+  <si>
+    <t>2023-06-27T13:40:17Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attualmente l'unica sezione opzionale gestita dall'applicativo è "Riscontri ed accertamenti significativi" mentre per il test case risultano essere tutti obbligatori.  </t>
   </si>
 </sst>
 </file>
@@ -1308,6 +1293,27 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1329,27 +1335,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1667,10 +1652,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="130.109375" customWidth="1"/>
-    <col min="2" max="26" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="130.140625" customWidth="1"/>
+    <col min="2" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="14.25" customHeight="1">
@@ -2733,11 +2718,11 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="194.109375" customWidth="1"/>
-    <col min="3" max="6" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="194.140625" customWidth="1"/>
+    <col min="3" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -2809,7 +2794,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="43.2">
+    <row r="11" spans="1:2" ht="45">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -3831,26 +3816,27 @@
   <dimension ref="A1:T646"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="46.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="63.88671875" customWidth="1"/>
-    <col min="5" max="5" width="104.88671875" customWidth="1"/>
-    <col min="6" max="9" width="33.109375" customWidth="1"/>
-    <col min="10" max="10" width="27.109375" customWidth="1"/>
-    <col min="11" max="15" width="36.44140625" customWidth="1"/>
-    <col min="16" max="16" width="27.109375" customWidth="1"/>
-    <col min="17" max="17" width="33.109375" customWidth="1"/>
-    <col min="18" max="18" width="36.44140625" customWidth="1"/>
-    <col min="19" max="20" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" customWidth="1"/>
+    <col min="5" max="5" width="104.85546875" customWidth="1"/>
+    <col min="6" max="8" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="11" max="15" width="36.42578125" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" customWidth="1"/>
+    <col min="17" max="17" width="33.140625" customWidth="1"/>
+    <col min="18" max="18" width="36.42578125" customWidth="1"/>
+    <col min="19" max="20" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -3871,15 +3857,15 @@
       <c r="S1" s="2"/>
       <c r="T1" s="15"/>
     </row>
-    <row r="2" spans="1:20" ht="18">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:20" ht="18.75">
+      <c r="A2" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="44"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3896,15 +3882,15 @@
       <c r="S2" s="2"/>
       <c r="T2" s="15"/>
     </row>
-    <row r="3" spans="1:20" ht="15.6">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:20" ht="15.75">
+      <c r="A3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="44"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3921,13 +3907,13 @@
       <c r="S3" s="2"/>
       <c r="T3" s="15"/>
     </row>
-    <row r="4" spans="1:20" ht="15.6">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="45" t="s">
+    <row r="4" spans="1:20" ht="15.75">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3945,13 +3931,13 @@
       <c r="S4" s="2"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="15.6">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45" t="s">
+    <row r="5" spans="1:20" ht="15.75">
+      <c r="A5" s="50"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3969,8 +3955,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4025,7 +4011,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="36.6" thickBot="1">
+    <row r="9" spans="1:20" ht="38.25" thickBot="1">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -4087,8 +4073,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="130.19999999999999" thickBot="1">
-      <c r="A10" s="47">
+    <row r="10" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A10" s="35">
         <v>6</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -4100,19 +4086,19 @@
       <c r="D10" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="36" t="s">
         <v>151</v>
       </c>
       <c r="F10" s="22">
-        <v>45097</v>
-      </c>
-      <c r="G10" s="52" t="s">
-        <v>177</v>
-      </c>
-      <c r="H10" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="I10" s="52" t="s">
+        <v>45104</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="I10" s="40" t="s">
         <v>172</v>
       </c>
       <c r="J10" s="24" t="s">
@@ -4131,8 +4117,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="130.19999999999999" thickBot="1">
-      <c r="A11" s="47">
+    <row r="11" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A11" s="35">
         <v>7</v>
       </c>
       <c r="B11" s="20" t="s">
@@ -4144,25 +4130,21 @@
       <c r="D11" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="36" t="s">
         <v>152</v>
       </c>
       <c r="F11" s="22">
-        <v>45097</v>
-      </c>
-      <c r="G11" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="H11" s="49" t="s">
-        <v>170</v>
-      </c>
-      <c r="I11" s="49" t="s">
-        <v>173</v>
-      </c>
+        <v>45104</v>
+      </c>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" s="24"/>
+        <v>146</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>175</v>
+      </c>
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
       <c r="N11" s="24"/>
@@ -4175,8 +4157,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="130.19999999999999" thickBot="1">
-      <c r="A12" s="47">
+    <row r="12" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A12" s="35">
         <v>8</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -4188,25 +4170,21 @@
       <c r="D12" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="36" t="s">
         <v>153</v>
       </c>
       <c r="F12" s="22">
-        <v>45097</v>
-      </c>
-      <c r="G12" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="H12" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="I12" s="49" t="s">
-        <v>174</v>
-      </c>
+        <v>45104</v>
+      </c>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="K12" s="24"/>
+        <v>146</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>175</v>
+      </c>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
@@ -4219,8 +4197,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="130.19999999999999" thickBot="1">
-      <c r="A13" s="47">
+    <row r="13" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A13" s="35">
         <v>9</v>
       </c>
       <c r="B13" s="20" t="s">
@@ -4239,10 +4217,10 @@
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="23"/>
-      <c r="J13" s="51" t="s">
+      <c r="J13" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="K13" s="51" t="s">
+      <c r="K13" s="39" t="s">
         <v>157</v>
       </c>
       <c r="L13" s="24"/>
@@ -4257,8 +4235,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="129.6">
-      <c r="A14" s="47">
+    <row r="14" spans="1:20" ht="150">
+      <c r="A14" s="35">
         <v>29</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -4277,10 +4255,10 @@
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
-      <c r="J14" s="51" t="s">
+      <c r="J14" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="39" t="s">
         <v>158</v>
       </c>
       <c r="L14" s="24"/>
@@ -4295,8 +4273,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="144.6" thickBot="1">
-      <c r="A15" s="47">
+    <row r="15" spans="1:20" ht="165.75" thickBot="1">
+      <c r="A15" s="35">
         <v>37</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -4308,17 +4286,17 @@
       <c r="D15" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="36" t="s">
         <v>63</v>
       </c>
       <c r="F15" s="22"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K15" s="51" t="s">
+      <c r="K15" s="39" t="s">
         <v>159</v>
       </c>
       <c r="L15" s="24"/>
@@ -4333,11 +4311,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="58.2" thickBot="1">
-      <c r="A16" s="47">
+    <row r="16" spans="1:20" ht="60.75" thickBot="1">
+      <c r="A16" s="35">
         <v>45</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="20" t="s">
@@ -4352,9 +4330,9 @@
       <c r="F16" s="22">
         <v>45097</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="24" t="s">
         <v>65</v>
       </c>
@@ -4365,13 +4343,13 @@
       <c r="M16" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="N16" s="50" t="s">
+      <c r="N16" s="38" t="s">
         <v>154</v>
       </c>
       <c r="O16" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="P16" s="51" t="s">
+      <c r="P16" s="39" t="s">
         <v>155</v>
       </c>
       <c r="Q16" s="24"/>
@@ -4381,14 +4359,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="115.8" thickBot="1">
-      <c r="A17" s="47">
+    <row r="17" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A17" s="35">
         <v>63</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="34" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="20" t="s">
@@ -4404,7 +4382,7 @@
       <c r="J17" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K17" s="51" t="s">
+      <c r="K17" s="39" t="s">
         <v>161</v>
       </c>
       <c r="L17" s="24"/>
@@ -4419,8 +4397,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="115.2">
-      <c r="A18" s="47">
+    <row r="18" spans="1:20" ht="120">
+      <c r="A18" s="35">
         <v>64</v>
       </c>
       <c r="B18" s="20" t="s">
@@ -4442,7 +4420,7 @@
       <c r="J18" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K18" s="51" t="s">
+      <c r="K18" s="39" t="s">
         <v>162</v>
       </c>
       <c r="L18" s="24"/>
@@ -4457,8 +4435,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="115.2">
-      <c r="A19" s="47">
+    <row r="19" spans="1:20" ht="120">
+      <c r="A19" s="35">
         <v>65</v>
       </c>
       <c r="B19" s="20" t="s">
@@ -4480,7 +4458,7 @@
       <c r="J19" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K19" s="51" t="s">
+      <c r="K19" s="39" t="s">
         <v>163</v>
       </c>
       <c r="L19" s="24"/>
@@ -4495,8 +4473,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="115.2">
-      <c r="A20" s="47">
+    <row r="20" spans="1:20" ht="120">
+      <c r="A20" s="35">
         <v>66</v>
       </c>
       <c r="B20" s="20" t="s">
@@ -4518,7 +4496,7 @@
       <c r="J20" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K20" s="51" t="s">
+      <c r="K20" s="39" t="s">
         <v>164</v>
       </c>
       <c r="L20" s="24"/>
@@ -4533,8 +4511,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="115.2">
-      <c r="A21" s="47">
+    <row r="21" spans="1:20" ht="120">
+      <c r="A21" s="35">
         <v>67</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -4556,7 +4534,7 @@
       <c r="J21" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K21" s="51" t="s">
+      <c r="K21" s="39" t="s">
         <v>165</v>
       </c>
       <c r="L21" s="24"/>
@@ -4571,8 +4549,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="115.2">
-      <c r="A22" s="47">
+    <row r="22" spans="1:20" ht="120">
+      <c r="A22" s="35">
         <v>68</v>
       </c>
       <c r="B22" s="20" t="s">
@@ -4594,7 +4572,7 @@
       <c r="J22" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K22" s="51" t="s">
+      <c r="K22" s="39" t="s">
         <v>166</v>
       </c>
       <c r="L22" s="24"/>
@@ -4609,8 +4587,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="115.2">
-      <c r="A23" s="47">
+    <row r="23" spans="1:20" ht="120">
+      <c r="A23" s="35">
         <v>69</v>
       </c>
       <c r="B23" s="20" t="s">
@@ -4632,7 +4610,7 @@
       <c r="J23" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K23" s="51" t="s">
+      <c r="K23" s="39" t="s">
         <v>160</v>
       </c>
       <c r="L23" s="24"/>
@@ -4647,8 +4625,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="115.2">
-      <c r="A24" s="47">
+    <row r="24" spans="1:20" ht="120">
+      <c r="A24" s="35">
         <v>70</v>
       </c>
       <c r="B24" s="20" t="s">
@@ -4670,7 +4648,7 @@
       <c r="J24" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K24" s="51" t="s">
+      <c r="K24" s="39" t="s">
         <v>160</v>
       </c>
       <c r="L24" s="24"/>
@@ -4685,8 +4663,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="115.2">
-      <c r="A25" s="47">
+    <row r="25" spans="1:20" ht="120">
+      <c r="A25" s="35">
         <v>71</v>
       </c>
       <c r="B25" s="20" t="s">
@@ -4708,7 +4686,7 @@
       <c r="J25" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K25" s="51" t="s">
+      <c r="K25" s="39" t="s">
         <v>167</v>
       </c>
       <c r="L25" s="24"/>
@@ -4723,8 +4701,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="115.2">
-      <c r="A26" s="47">
+    <row r="26" spans="1:20" ht="120">
+      <c r="A26" s="35">
         <v>72</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -4746,7 +4724,7 @@
       <c r="J26" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K26" s="51" t="s">
+      <c r="K26" s="39" t="s">
         <v>168</v>
       </c>
       <c r="L26" s="24"/>
@@ -4761,8 +4739,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="115.2">
-      <c r="A27" s="47">
+    <row r="27" spans="1:20" ht="120">
+      <c r="A27" s="35">
         <v>73</v>
       </c>
       <c r="B27" s="20" t="s">
@@ -4784,7 +4762,7 @@
       <c r="J27" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K27" s="51" t="s">
+      <c r="K27" s="39" t="s">
         <v>168</v>
       </c>
       <c r="L27" s="24"/>
@@ -4799,8 +4777,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="115.8" thickBot="1">
-      <c r="A28" s="47">
+    <row r="28" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A28" s="35">
         <v>74</v>
       </c>
       <c r="B28" s="20" t="s">
@@ -4822,7 +4800,7 @@
       <c r="J28" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="K28" s="51" t="s">
+      <c r="K28" s="39" t="s">
         <v>168</v>
       </c>
       <c r="L28" s="24"/>
@@ -4837,14 +4815,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="129.6">
-      <c r="A29" s="47">
+    <row r="29" spans="1:20" ht="150">
+      <c r="A29" s="35">
         <v>369</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="34" t="s">
         <v>47</v>
       </c>
       <c r="D29" s="33" t="s">
@@ -4856,14 +4834,14 @@
       <c r="F29" s="22">
         <v>45097</v>
       </c>
-      <c r="G29" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="H29" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="I29" s="49" t="s">
-        <v>176</v>
+      <c r="G29" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="H29" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="I29" s="37" t="s">
+        <v>170</v>
       </c>
       <c r="J29" s="24" t="s">
         <v>65</v>
@@ -9586,13 +9564,13 @@
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="102" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -9679,7 +9657,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.4" hidden="1">
+    <row r="7" spans="1:4" hidden="1">
       <c r="A7" s="11" t="s">
         <v>56</v>
       </c>
@@ -9693,7 +9671,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.4" hidden="1">
+    <row r="8" spans="1:4" hidden="1">
       <c r="A8" s="11" t="s">
         <v>61</v>
       </c>
@@ -9707,7 +9685,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.4" hidden="1">
+    <row r="9" spans="1:4" hidden="1">
       <c r="A9" s="11" t="s">
         <v>60</v>
       </c>
@@ -9721,7 +9699,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.2" hidden="1">
+    <row r="10" spans="1:4" ht="45" hidden="1">
       <c r="A10" s="11" t="s">
         <v>112</v>
       </c>
@@ -11264,11 +11242,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="6" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>